<commit_message>
near-final run successful (with minor syntax fix)
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Range Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority Status" sheetId="3" r:id="rId3"/>
     <sheet name="Species qualification" sheetId="4" r:id="rId4"/>
+    <sheet name="SoIB-IUCN cross-tab" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -384,7 +385,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>64</v>
@@ -397,7 +398,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3">
         <v>78</v>
@@ -410,10 +411,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>333</v>
+        <v>425</v>
       </c>
       <c r="C4">
-        <v>213</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5">
@@ -423,7 +424,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C5">
         <v>284</v>
@@ -436,7 +437,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C6">
         <v>189</v>
@@ -449,7 +450,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>17</v>
@@ -462,7 +463,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -510,7 +511,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -520,7 +521,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>160</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5">
@@ -530,7 +531,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>341</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6">
@@ -585,7 +586,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3">
@@ -595,7 +596,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>271</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4">
@@ -605,7 +606,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>397</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -640,7 +641,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>856</v>
+        <v>948</v>
       </c>
     </row>
     <row r="3">
@@ -650,7 +651,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>524</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4">
@@ -660,7 +661,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>644</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5">
@@ -670,7 +671,180 @@
         </is>
       </c>
       <c r="B5">
-        <v>856</v>
+        <v>948</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Critically Endangered</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Endangered</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Vulnerable</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Near Threatened</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Least Concern</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>105</v>
+      </c>
+      <c r="C6">
+        <v>297</v>
+      </c>
+      <c r="D6">
+        <v>387</v>
+      </c>
+      <c r="E6">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Not Recognised</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>204</v>
+      </c>
+      <c r="C8">
+        <v>404</v>
+      </c>
+      <c r="D8">
+        <v>340</v>
+      </c>
+      <c r="E8">
+        <v>948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run after correcting for Violet Cuckoo and Fire-capped Tit. Also island restricted birds.
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -385,10 +385,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -398,10 +398,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -411,10 +411,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C4">
-        <v>305</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5">
@@ -424,10 +424,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C5">
-        <v>284</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6">
@@ -437,10 +437,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C6">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7">
@@ -453,7 +453,7 @@
         <v>19</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -466,7 +466,7 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>231</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>204</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="3">
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>650</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5">
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -778,10 +778,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -797,16 +797,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C6">
-        <v>297</v>
+        <v>327</v>
       </c>
       <c r="D6">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E6">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="7">
@@ -816,10 +816,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -835,16 +835,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="C8">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D8">
-        <v>340</v>
+        <v>385</v>
       </c>
       <c r="E8">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run after correcting NAs
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -385,10 +385,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -398,10 +398,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
@@ -411,10 +411,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C4">
-        <v>284</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5">
@@ -424,10 +424,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6">
@@ -437,10 +437,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7">
@@ -453,7 +453,7 @@
         <v>19</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -466,7 +466,7 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>298</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>385</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>673</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5">
@@ -778,10 +778,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -797,13 +797,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C6">
-        <v>327</v>
+        <v>299</v>
       </c>
       <c r="D6">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E6">
         <v>787</v>
@@ -816,10 +816,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="C8">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D8">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="E8">
         <v>946</v>

</xml_diff>

<commit_message>
One more run after removing Brown-crowned Scimitar-Babbler
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -411,10 +411,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C4">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3">
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="3">
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
   </sheetData>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>299</v>
@@ -806,7 +806,7 @@
         <v>387</v>
       </c>
       <c r="E6">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="7">
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8">
         <v>404</v>
@@ -844,7 +844,7 @@
         <v>343</v>
       </c>
       <c r="E8">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After the final full country run
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -407,20 +407,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>eBird Data Deficient</t>
+          <t>Insufficient Data</t>
         </is>
       </c>
       <c r="B4">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C4">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>eBird Data Inconclusive</t>
+          <t>Trend Inconclusive</t>
         </is>
       </c>
       <c r="B5">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5">
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>348</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>110</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>343</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>404</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="3">
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -759,10 +759,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -778,10 +778,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -797,13 +797,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C6">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="D6">
-        <v>387</v>
+        <v>423</v>
       </c>
       <c r="E6">
         <v>786</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -835,16 +835,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="C8">
-        <v>404</v>
+        <v>441</v>
       </c>
       <c r="D8">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="E8">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more summaries into the summaries, made a small correction to the main file, where the Long-Term.Analysis column is synced with Insufficient Data
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -11,7 +11,14 @@
     <sheet name="Range Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority Status" sheetId="3" r:id="rId3"/>
     <sheet name="Species qualification" sheetId="4" r:id="rId4"/>
-    <sheet name="SoIB-IUCN cross-tab" sheetId="5" r:id="rId5"/>
+    <sheet name="SoIB 2020 to 2023 comparison" sheetId="5" r:id="rId5"/>
+    <sheet name="SoIB 2023 to 2020 comparison" sheetId="6" r:id="rId6"/>
+    <sheet name="SoIB-IUCN cross-tab" sheetId="7" r:id="rId7"/>
+    <sheet name="SoIB-IUCN percentage IUCN" sheetId="8" r:id="rId8"/>
+    <sheet name="SoIB-IUCN percentage SoIB" sheetId="9" r:id="rId9"/>
+    <sheet name="High Priority break up" sheetId="10" r:id="rId10"/>
+    <sheet name="Reason for uplisting" sheetId="11" r:id="rId11"/>
+    <sheet name="Reason for downlisting" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -355,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,6 +384,16 @@
           <t>Current species</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of species with conclusive ltt</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of species with conclusive ct</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -390,6 +407,12 @@
       <c r="C2">
         <v>64</v>
       </c>
+      <c r="D2">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>17.8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -403,70 +426,485 @@
       <c r="C3">
         <v>78</v>
       </c>
+      <c r="D3">
+        <v>31.4</v>
+      </c>
+      <c r="E3">
+        <v>21.7</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Insufficient Data</t>
+          <t>Stable</t>
         </is>
       </c>
       <c r="B4">
-        <v>419</v>
+        <v>98</v>
       </c>
       <c r="C4">
-        <v>299</v>
+        <v>189</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>52.6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Trend Inconclusive</t>
+          <t>Increase</t>
         </is>
       </c>
       <c r="B5">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>284</v>
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>5.6</v>
+      </c>
+      <c r="E5">
+        <v>4.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Stable</t>
+          <t>Rapid Increase</t>
         </is>
       </c>
       <c r="B6">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>189</v>
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Insufficient Data</t>
         </is>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>419</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rapid Increase</t>
+          <t>Trend Inconclusive</t>
         </is>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Break-up</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>No. of High species</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of High species</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>No. of new High species in SoIB 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of new High species</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Trend</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>52.8</v>
+      </c>
+      <c r="D2">
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Range</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>25.3</v>
+      </c>
+      <c r="D3">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IUCN</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>21.9</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>3.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Break-up</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>No. of species</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of species</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>First-time trend</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>More decline in ltt</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>More decline in ct</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>First-time ltt</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>First-time ct</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other changes in trends</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Loss of trends</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Reducing range</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Break-up</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>No. of species</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of species</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Less decline in ltt</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Less decline in ct</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>First-time trend</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>First-time ltt</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>First-time ct</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other changes in trends</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Loss of trends</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Increasing range</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +914,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -493,6 +931,11 @@
           <t>No. of species</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -503,6 +946,9 @@
       <c r="B2">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -513,6 +959,9 @@
       <c r="B3">
         <v>46</v>
       </c>
+      <c r="C3">
+        <v>4.9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -523,6 +972,9 @@
       <c r="B4">
         <v>220</v>
       </c>
+      <c r="C4">
+        <v>23.4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -533,6 +985,9 @@
       <c r="B5">
         <v>363</v>
       </c>
+      <c r="C5">
+        <v>38.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -543,6 +998,9 @@
       <c r="B6">
         <v>178</v>
       </c>
+      <c r="C6">
+        <v>18.9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -552,6 +1010,9 @@
       </c>
       <c r="B7">
         <v>131</v>
+      </c>
+      <c r="C7">
+        <v>13.9</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +1077,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -633,6 +1094,11 @@
           <t>No. of species</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>No. of species with conclusive trends</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -651,7 +1117,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>530</v>
+        <v>523</v>
+      </c>
+      <c r="C3">
+        <v>338</v>
       </c>
     </row>
     <row r="4">
@@ -661,7 +1130,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>650</v>
+        <v>643</v>
+      </c>
+      <c r="C4">
+        <v>359</v>
       </c>
     </row>
     <row r="5">
@@ -680,6 +1152,478 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SOIB Concern Status</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SOIBv2 Priority Status</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>No. of species</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of species</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>74</v>
+      </c>
+      <c r="D2">
+        <v>73.3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>333</v>
+      </c>
+      <c r="D7">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>72</v>
+      </c>
+      <c r="D8">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>81</v>
+      </c>
+      <c r="D11">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>166</v>
+      </c>
+      <c r="D12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SOIBv2 Priority Status</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SOIB Concern Status</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>No. of species</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Perc. of species</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>74</v>
+      </c>
+      <c r="D2">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>56</v>
+      </c>
+      <c r="D4">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>333</v>
+      </c>
+      <c r="D7">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>81</v>
+      </c>
+      <c r="D8">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>72</v>
+      </c>
+      <c r="D11">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>166</v>
+      </c>
+      <c r="D12">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>63</v>
+      </c>
+      <c r="D13">
+        <v>19.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -838,13 +1782,286 @@
         <v>178</v>
       </c>
       <c r="C8">
+        <v>323</v>
+      </c>
+      <c r="D8">
         <v>441</v>
-      </c>
-      <c r="D8">
-        <v>323</v>
       </c>
       <c r="E8">
         <v>942</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Critically Endangered</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Endangered</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>93.8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>6.2</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Vulnerable</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>80.8</v>
+      </c>
+      <c r="C4">
+        <v>15.4</v>
+      </c>
+      <c r="D4">
+        <v>3.8</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Near Threatened</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>25.4</v>
+      </c>
+      <c r="C5">
+        <v>58.2</v>
+      </c>
+      <c r="D5">
+        <v>16.4</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Least Concern</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>11.5</v>
+      </c>
+      <c r="C6">
+        <v>34.6</v>
+      </c>
+      <c r="D6">
+        <v>53.9</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Not Recognised</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Critically Endangered</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Endangered</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Vulnerable</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Near Threatened</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Least Concern</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Not Recognised</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>7.9</v>
+      </c>
+      <c r="B2">
+        <v>8.4</v>
+      </c>
+      <c r="C2">
+        <v>23.6</v>
+      </c>
+      <c r="D2">
+        <v>9.6</v>
+      </c>
+      <c r="E2">
+        <v>50.6</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2.5</v>
+      </c>
+      <c r="D3">
+        <v>12.1</v>
+      </c>
+      <c r="E3">
+        <v>84.2</v>
+      </c>
+      <c r="F3">
+        <v>1.2</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+      <c r="E4">
+        <v>95.90000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a correction to the summary file and created the 'growth' graph
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -408,10 +408,10 @@
         <v>64</v>
       </c>
       <c r="D2">
-        <v>29</v>
+        <v>28.4</v>
       </c>
       <c r="E2">
-        <v>17.8</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="3">
@@ -427,10 +427,10 @@
         <v>78</v>
       </c>
       <c r="D3">
-        <v>31.4</v>
+        <v>30.7</v>
       </c>
       <c r="E3">
-        <v>21.7</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="4">
@@ -446,10 +446,10 @@
         <v>189</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>28.4</v>
       </c>
       <c r="E4">
-        <v>52.6</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="5">
@@ -465,10 +465,10 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="E5">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="6">
@@ -484,10 +484,10 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="E6">
-        <v>3.1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -559,57 +559,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Trend</t>
+          <t>Trend New</t>
         </is>
       </c>
       <c r="B2">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C2">
-        <v>52.8</v>
+        <v>43.3</v>
       </c>
       <c r="D2">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E2">
-        <v>75</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Range</t>
+          <t>Trend Different</t>
         </is>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>25.3</v>
+        <v>9.6</v>
       </c>
       <c r="D3">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>21.2</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Range</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>25.3</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>IUCN</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>39</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>21.9</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>3.8</v>
       </c>
     </row>
@@ -797,10 +816,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -810,10 +829,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -862,10 +881,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -1117,10 +1136,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="C3">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
@@ -1130,10 +1149,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>643</v>
+        <v>650</v>
       </c>
       <c r="C4">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
cleaned latest summaries code
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Range Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority Status" sheetId="3" r:id="rId3"/>
     <sheet name="Species qualification" sheetId="4" r:id="rId4"/>
-    <sheet name="SoIB 2020 to 2023 comparison" sheetId="5" r:id="rId5"/>
-    <sheet name="SoIB 2023 to 2020 comparison" sheetId="6" r:id="rId6"/>
-    <sheet name="SoIB-IUCN cross-tab" sheetId="7" r:id="rId7"/>
-    <sheet name="SoIB-IUCN percentage IUCN" sheetId="8" r:id="rId8"/>
-    <sheet name="SoIB-IUCN percentage SoIB" sheetId="9" r:id="rId9"/>
-    <sheet name="High Priority break up" sheetId="10" r:id="rId10"/>
+    <sheet name="SoIB 2020 vs 2023" sheetId="5" r:id="rId5"/>
+    <sheet name="SoIB 2023 vs 2020" sheetId="6" r:id="rId6"/>
+    <sheet name="SoIB vs IUCN (no.)" sheetId="7" r:id="rId7"/>
+    <sheet name="SoIB vs IUCN (IUCN %)" sheetId="8" r:id="rId8"/>
+    <sheet name="SoIB vs IUCN (SoIB %)" sheetId="9" r:id="rId9"/>
+    <sheet name="High Priority break-up" sheetId="10" r:id="rId10"/>
     <sheet name="Reason for uplisting" sheetId="11" r:id="rId11"/>
     <sheet name="Reason for downlisting" sheetId="12" r:id="rId12"/>
   </sheets>
@@ -376,22 +376,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Long-term species</t>
+          <t>Long-term species (no.)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Current species</t>
+          <t>Current species (no.)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of species with conclusive ltt</t>
+          <t>Long-term species conclusive (perc.)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of species with conclusive ct</t>
+          <t>Current species conclusive (perc.)</t>
         </is>
       </c>
     </row>
@@ -493,27 +493,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Insufficient Data</t>
+          <t>Trend Inconclusive</t>
         </is>
       </c>
       <c r="B7">
-        <v>419</v>
+        <v>185</v>
       </c>
       <c r="C7">
-        <v>299</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Trend Inconclusive</t>
+          <t>Insufficient Data</t>
         </is>
       </c>
       <c r="B8">
-        <v>185</v>
+        <v>419</v>
       </c>
       <c r="C8">
-        <v>284</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -537,22 +537,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>No. of High species</t>
+          <t>High Species (no.)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of High species</t>
+          <t>High Species (perc.)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>No. of new High species in SoIB 2023</t>
+          <t>New High Species (no.)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of new High species</t>
+          <t>New High Species (perc.)</t>
         </is>
       </c>
     </row>
@@ -653,58 +653,58 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>No. of species</t>
+          <t>Species (no.)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of species</t>
+          <t>Species (perc.)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>First-time trend</t>
+          <t>More decline in LTT</t>
         </is>
       </c>
       <c r="B2">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>36.4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>More decline in ltt</t>
+          <t>More decline in CAT</t>
         </is>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>More decline in ct</t>
+          <t>First-time trend</t>
         </is>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>First-time ltt</t>
+          <t>First-time LTT</t>
         </is>
       </c>
       <c r="B5">
@@ -717,7 +717,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>First-time ct</t>
+          <t>First-time CAT</t>
         </is>
       </c>
       <c r="B6">
@@ -800,19 +800,19 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>No. of species</t>
+          <t>Species (no.)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of species</t>
+          <t>Species (perc.)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Less decline in ltt</t>
+          <t>Less decline in LTT</t>
         </is>
       </c>
       <c r="B2">
@@ -825,7 +825,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Less decline in ct</t>
+          <t>Less decline in CAT</t>
         </is>
       </c>
       <c r="B3">
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>First-time ltt</t>
+          <t>First-time LTT</t>
         </is>
       </c>
       <c r="B5">
@@ -864,14 +864,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>First-time ct</t>
+          <t>First-time CAT</t>
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -947,12 +947,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>No. of species</t>
+          <t>Species (no.)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of total</t>
+          <t>Species (perc.)</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Selected for:</t>
+          <t>No. of species in:</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>No. of species</t>
+          <t>Selected for analysis</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>No. of species with conclusive trends</t>
+          <t>With conclusive trends</t>
         </is>
       </c>
     </row>
@@ -1191,12 +1191,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>No. of species</t>
+          <t>Species (no.)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of species</t>
+          <t>Species (perc.)</t>
         </is>
       </c>
     </row>
@@ -1427,12 +1427,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>No. of species</t>
+          <t>Species (no.)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Perc. of species</t>
+          <t>Species (perc.)</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1844,11 +1844,6 @@
           <t>Low</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Sum</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1865,9 +1860,6 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1884,9 +1876,6 @@
       <c r="D3">
         <v>6.2</v>
       </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1903,9 +1892,6 @@
       <c r="D4">
         <v>3.8</v>
       </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1922,9 +1908,6 @@
       <c r="D5">
         <v>16.4</v>
       </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1941,9 +1924,6 @@
       <c r="D6">
         <v>53.9</v>
       </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1959,9 +1939,6 @@
       </c>
       <c r="D7">
         <v>50</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1980,107 +1957,113 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Critically Endangered</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Endangered</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Vulnerable</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Near Threatened</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Least Concern</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Not Recognised</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Sum</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B2">
         <v>7.9</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>8.4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>23.6</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>9.6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>50.6</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>0</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>2.5</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>12.1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>84.2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1.2</v>
       </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.2</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2.5</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>95.90000000000001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.9</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolve debug: partial runs completed
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Range Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority Status" sheetId="3" r:id="rId3"/>
     <sheet name="Species qualification" sheetId="4" r:id="rId4"/>
-    <sheet name="SoIB 2020 vs 2023" sheetId="5" r:id="rId5"/>
-    <sheet name="SoIB 2023 vs 2020" sheetId="6" r:id="rId6"/>
-    <sheet name="SoIB vs IUCN (no.)" sheetId="7" r:id="rId7"/>
-    <sheet name="SoIB vs IUCN (IUCN %)" sheetId="8" r:id="rId8"/>
-    <sheet name="SoIB vs IUCN (SoIB %)" sheetId="9" r:id="rId9"/>
-    <sheet name="High Priority break-up" sheetId="10" r:id="rId10"/>
+    <sheet name="High Priority break-up" sheetId="5" r:id="rId5"/>
+    <sheet name="SoIB 2020 vs 2023" sheetId="6" r:id="rId6"/>
+    <sheet name="SoIB 2023 vs 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="SoIB vs IUCN (no.)" sheetId="8" r:id="rId8"/>
+    <sheet name="SoIB vs IUCN (IUCN %)" sheetId="9" r:id="rId9"/>
+    <sheet name="SoIB vs IUCN (SoIB %)" sheetId="10" r:id="rId10"/>
     <sheet name="Reason for uplisting" sheetId="11" r:id="rId11"/>
     <sheet name="Reason for downlisting" sheetId="12" r:id="rId12"/>
   </sheets>
@@ -402,16 +402,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>64</v>
       </c>
       <c r="D2">
-        <v>28.4</v>
+        <v>28.2</v>
       </c>
       <c r="E2">
-        <v>17.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -421,16 +421,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <v>78</v>
       </c>
       <c r="D3">
-        <v>30.7</v>
+        <v>30.4</v>
       </c>
       <c r="E3">
-        <v>21.3</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="4">
@@ -440,16 +440,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D4">
-        <v>28.4</v>
+        <v>31</v>
       </c>
       <c r="E4">
-        <v>51.6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -459,16 +459,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>17</v>
       </c>
       <c r="D5">
-        <v>5.5</v>
+        <v>6.3</v>
       </c>
       <c r="E5">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="6">
@@ -478,16 +478,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>4.9</v>
+        <v>4.1</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="7">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="C7">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8">
@@ -523,7 +523,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,104 +532,113 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Break-up</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>High Species (no.)</t>
+          <t>Critically Endangered</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>High Species (perc.)</t>
+          <t>Endangered</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>New High Species (no.)</t>
+          <t>Vulnerable</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>New High Species (perc.)</t>
+          <t>Near Threatened</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Least Concern</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Not Recognised</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Trend New</t>
+          <t>High</t>
         </is>
       </c>
       <c r="B2">
-        <v>77</v>
+        <v>8.1</v>
       </c>
       <c r="C2">
-        <v>43.3</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="D2">
-        <v>71</v>
+        <v>24.3</v>
       </c>
       <c r="E2">
-        <v>68.3</v>
+        <v>9.800000000000001</v>
+      </c>
+      <c r="F2">
+        <v>49.1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Trend Different</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>9.6</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>2.5</v>
       </c>
       <c r="E3">
-        <v>6.7</v>
+        <v>12.4</v>
+      </c>
+      <c r="F3">
+        <v>82.8</v>
+      </c>
+      <c r="G3">
+        <v>2.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Range</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="B4">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>25.3</v>
+        <v>0.2</v>
       </c>
       <c r="D4">
-        <v>22</v>
+        <v>0.4</v>
       </c>
       <c r="E4">
-        <v>21.2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>IUCN</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>39</v>
-      </c>
-      <c r="C5">
-        <v>21.9</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>3.8</v>
+        <v>2.4</v>
+      </c>
+      <c r="F4">
+        <v>95.8</v>
+      </c>
+      <c r="G4">
+        <v>1.1</v>
       </c>
     </row>
   </sheetData>
@@ -669,10 +678,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="3">
@@ -698,7 +707,7 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>36.4</v>
+        <v>38.6</v>
       </c>
     </row>
     <row r="5">
@@ -711,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2.3</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="6">
@@ -721,10 +730,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>22.7</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="7">
@@ -737,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8">
@@ -750,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9">
@@ -763,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>11.4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -816,10 +825,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -829,10 +838,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -1066,7 +1075,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3">
@@ -1076,7 +1085,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
@@ -1086,7 +1095,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>441</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -1136,10 +1145,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C3">
-        <v>345</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4">
@@ -1149,10 +1158,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="C4">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
@@ -1172,7 +1181,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1181,224 +1190,104 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SOIB Concern Status</t>
+          <t>Break-up</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>SOIBv2 Priority Status</t>
+          <t>High Species (no.)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Species (no.)</t>
+          <t>High Species (perc.)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Species (perc.)</t>
+          <t>New High Species (no.)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>New High Species (perc.)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+          <t>Trend New</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>73</v>
       </c>
       <c r="C2">
-        <v>74</v>
+        <v>42.2</v>
       </c>
       <c r="D2">
-        <v>73.3</v>
+        <v>67</v>
+      </c>
+      <c r="E2">
+        <v>67.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+          <t>Trend Different</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>6.1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+          <t>Range</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>45</v>
       </c>
       <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>21.8</v>
+      <c r="E4">
+        <v>22.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
+          <t>IUCN</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>39</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>22.5</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="C6">
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>333</v>
-      </c>
-      <c r="D7">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>72</v>
-      </c>
-      <c r="D8">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>56</v>
-      </c>
-      <c r="D10">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>81</v>
-      </c>
-      <c r="D11">
-        <v>25.4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>166</v>
-      </c>
-      <c r="D12">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
+      <c r="E5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1417,12 +1306,12 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>SOIB Concern Status</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>SOIBv2 Priority Status</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>SOIB Concern Status</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1451,7 +1340,7 @@
         <v>74</v>
       </c>
       <c r="D2">
-        <v>41.6</v>
+        <v>73.3</v>
       </c>
     </row>
     <row r="3">
@@ -1466,10 +1355,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="4">
@@ -1484,10 +1373,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>31.5</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="5">
@@ -1497,10 +1386,10 @@
         </is>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1515,10 +1404,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D6">
-        <v>0.7</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="7">
@@ -1533,10 +1422,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D7">
-        <v>75.5</v>
+        <v>75.3</v>
       </c>
     </row>
     <row r="8">
@@ -1551,10 +1440,10 @@
         </is>
       </c>
       <c r="C8">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D8">
-        <v>18.4</v>
+        <v>16.6</v>
       </c>
     </row>
     <row r="9">
@@ -1564,10 +1453,10 @@
         </is>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>5.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10">
@@ -1582,10 +1471,10 @@
         </is>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D10">
-        <v>6.8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -1600,10 +1489,10 @@
         </is>
       </c>
       <c r="C11">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="D11">
-        <v>22.3</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="12">
@@ -1618,10 +1507,10 @@
         </is>
       </c>
       <c r="C12">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D12">
-        <v>51.4</v>
+        <v>49.8</v>
       </c>
     </row>
     <row r="13">
@@ -1631,10 +1520,10 @@
         </is>
       </c>
       <c r="C13">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="D13">
-        <v>19.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1643,6 +1532,242 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SOIBv2 Priority Status</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SOIB Concern Status</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Species (no.)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Species (perc.)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>74</v>
+      </c>
+      <c r="D2">
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>51</v>
+      </c>
+      <c r="D4">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>9.199999999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>332</v>
+      </c>
+      <c r="D7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>73</v>
+      </c>
+      <c r="D11">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>159</v>
+      </c>
+      <c r="D12">
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Moderate</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>63</v>
+      </c>
+      <c r="D13">
+        <v>20.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1760,16 +1885,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C6">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D6">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="E6">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7">
@@ -1782,13 +1907,13 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -1798,13 +1923,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C8">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D8">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="E8">
         <v>942</v>
@@ -1815,7 +1940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1916,13 +2041,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>11.5</v>
+        <v>10.9</v>
       </c>
       <c r="C6">
-        <v>34.6</v>
+        <v>33.3</v>
       </c>
       <c r="D6">
-        <v>53.9</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="7">
@@ -1935,135 +2060,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>58.3</v>
       </c>
       <c r="D7">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Critically Endangered</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Endangered</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Vulnerable</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Near Threatened</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Least Concern</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Not Recognised</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>7.9</v>
-      </c>
-      <c r="C2">
-        <v>8.4</v>
-      </c>
-      <c r="D2">
-        <v>23.6</v>
-      </c>
-      <c r="E2">
-        <v>9.6</v>
-      </c>
-      <c r="F2">
-        <v>50.6</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>2.5</v>
-      </c>
-      <c r="E3">
-        <v>12.1</v>
-      </c>
-      <c r="F3">
-        <v>84.2</v>
-      </c>
-      <c r="G3">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>2.5</v>
-      </c>
-      <c r="F4">
-        <v>95.90000000000001</v>
-      </c>
-      <c r="G4">
-        <v>0.9</v>
+        <v>41.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FINAL resolve and classification
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -402,16 +402,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>64</v>
       </c>
       <c r="D2">
-        <v>28.2</v>
+        <v>29</v>
       </c>
       <c r="E2">
-        <v>18</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="3">
@@ -421,16 +421,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C3">
         <v>78</v>
       </c>
       <c r="D3">
-        <v>30.4</v>
+        <v>31.4</v>
       </c>
       <c r="E3">
-        <v>21.9</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="4">
@@ -440,16 +440,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D4">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4">
-        <v>52</v>
+        <v>52.6</v>
       </c>
     </row>
     <row r="5">
@@ -459,16 +459,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>17</v>
       </c>
       <c r="D5">
-        <v>6.3</v>
+        <v>5.6</v>
       </c>
       <c r="E5">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="6">
@@ -478,16 +478,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>4.1</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="7">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="C7">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8">
@@ -573,19 +573,19 @@
         </is>
       </c>
       <c r="B2">
-        <v>8.1</v>
+        <v>7.9</v>
       </c>
       <c r="C2">
-        <v>8.699999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="D2">
-        <v>24.3</v>
+        <v>23.6</v>
       </c>
       <c r="E2">
-        <v>9.800000000000001</v>
+        <v>9.6</v>
       </c>
       <c r="F2">
-        <v>49.1</v>
+        <v>50.6</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -607,10 +607,10 @@
         <v>2.5</v>
       </c>
       <c r="E3">
-        <v>12.4</v>
+        <v>12.1</v>
       </c>
       <c r="F3">
-        <v>82.8</v>
+        <v>83.3</v>
       </c>
       <c r="G3">
         <v>2.2</v>
@@ -629,13 +629,13 @@
         <v>0.2</v>
       </c>
       <c r="D4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="F4">
-        <v>95.8</v>
+        <v>95.7</v>
       </c>
       <c r="G4">
         <v>1.1</v>
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>25.3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -707,7 +707,7 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>38.6</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="5">
@@ -720,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="6">
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>19.3</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="8">
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="9">
@@ -772,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="10">
@@ -825,10 +825,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>314</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>455</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1148,7 @@
         <v>523</v>
       </c>
       <c r="C3">
-        <v>319</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
@@ -1161,7 +1161,7 @@
         <v>643</v>
       </c>
       <c r="C4">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5">
@@ -1221,16 +1221,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C2">
-        <v>42.2</v>
+        <v>43.3</v>
       </c>
       <c r="D2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E2">
-        <v>67.7</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="3">
@@ -1240,16 +1240,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>9.199999999999999</v>
+        <v>9.6</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="4">
@@ -1262,13 +1262,13 @@
         <v>45</v>
       </c>
       <c r="C4">
-        <v>26</v>
+        <v>25.3</v>
       </c>
       <c r="D4">
         <v>22</v>
       </c>
       <c r="E4">
-        <v>22.2</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="5">
@@ -1281,13 +1281,13 @@
         <v>39</v>
       </c>
       <c r="C5">
-        <v>22.5</v>
+        <v>21.9</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>5.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -1373,10 +1373,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>18.8</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="5">
@@ -1422,10 +1422,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D7">
-        <v>75.3</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="8">
@@ -1440,10 +1440,10 @@
         </is>
       </c>
       <c r="C8">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8">
-        <v>16.6</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="9">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="C10">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D10">
-        <v>16</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="11">
@@ -1489,10 +1489,10 @@
         </is>
       </c>
       <c r="C11">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D11">
-        <v>29.2</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="12">
@@ -1507,10 +1507,10 @@
         </is>
       </c>
       <c r="C12">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D12">
-        <v>49.8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
@@ -1576,7 +1576,7 @@
         <v>74</v>
       </c>
       <c r="D2">
-        <v>42.8</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="3">
@@ -1594,7 +1594,7 @@
         <v>32</v>
       </c>
       <c r="D3">
-        <v>18.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -1609,10 +1609,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4">
-        <v>29.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="5">
@@ -1625,7 +1625,7 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -1640,10 +1640,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="7">
@@ -1658,10 +1658,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D7">
-        <v>73</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="8">
@@ -1676,10 +1676,10 @@
         </is>
       </c>
       <c r="C8">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D8">
-        <v>20.4</v>
+        <v>18.4</v>
       </c>
     </row>
     <row r="9">
@@ -1692,7 +1692,7 @@
         <v>24</v>
       </c>
       <c r="D9">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="10">
@@ -1707,10 +1707,10 @@
         </is>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>6.1</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="11">
@@ -1725,10 +1725,10 @@
         </is>
       </c>
       <c r="C11">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
-        <v>23.2</v>
+        <v>22.3</v>
       </c>
     </row>
     <row r="12">
@@ -1743,10 +1743,10 @@
         </is>
       </c>
       <c r="C12">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D12">
-        <v>50.6</v>
+        <v>51.4</v>
       </c>
     </row>
     <row r="13">
@@ -1759,7 +1759,7 @@
         <v>63</v>
       </c>
       <c r="D13">
-        <v>20.1</v>
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>
@@ -1885,13 +1885,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C6">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D6">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="E6">
         <v>781</v>
@@ -1923,13 +1923,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C8">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="D8">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="E8">
         <v>942</v>
@@ -2041,13 +2041,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>10.9</v>
+        <v>11.5</v>
       </c>
       <c r="C6">
-        <v>33.3</v>
+        <v>34.4</v>
       </c>
       <c r="D6">
-        <v>55.8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
After addressing annotations and creating scripts for the methods papers
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f61412a3b6644a5d/Documents/GitHub/soib_v2/01_analyses_full/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_731CB15E13ABE5F5B7A6A05411BB4C0B1FE5DA23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50130536-ED49-440D-8F35-3199A8212709}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trends Status" sheetId="1" r:id="rId1"/>
@@ -20,13 +26,207 @@
     <sheet name="Reason for uplisting" sheetId="11" r:id="rId11"/>
     <sheet name="Reason for downlisting" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+  <si>
+    <t>Trend Status</t>
+  </si>
+  <si>
+    <t>Long-term species (no.)</t>
+  </si>
+  <si>
+    <t>Current species (no.)</t>
+  </si>
+  <si>
+    <t>Long-term species conclusive (perc.)</t>
+  </si>
+  <si>
+    <t>Current species conclusive (perc.)</t>
+  </si>
+  <si>
+    <t>Rapid Decline</t>
+  </si>
+  <si>
+    <t>Decline</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
+  <si>
+    <t>Rapid Increase</t>
+  </si>
+  <si>
+    <t>Trend Inconclusive</t>
+  </si>
+  <si>
+    <t>Insufficient Data</t>
+  </si>
+  <si>
+    <t>Range Status</t>
+  </si>
+  <si>
+    <t>Species (no.)</t>
+  </si>
+  <si>
+    <t>Species (perc.)</t>
+  </si>
+  <si>
+    <t>Historical</t>
+  </si>
+  <si>
+    <t>Very Restricted</t>
+  </si>
+  <si>
+    <t>Restricted</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Very Large</t>
+  </si>
+  <si>
+    <t>Priority Status</t>
+  </si>
+  <si>
+    <t>No. of species</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>No. of species in:</t>
+  </si>
+  <si>
+    <t>Selected for analysis</t>
+  </si>
+  <si>
+    <t>With conclusive trends</t>
+  </si>
+  <si>
+    <t>SoIB 2023 Assessment</t>
+  </si>
+  <si>
+    <t>Long-term Analysis</t>
+  </si>
+  <si>
+    <t>Current Analysis</t>
+  </si>
+  <si>
+    <t>Range Analysis</t>
+  </si>
+  <si>
+    <t>Break-up</t>
+  </si>
+  <si>
+    <t>High Species (no.)</t>
+  </si>
+  <si>
+    <t>High Species (perc.)</t>
+  </si>
+  <si>
+    <t>New High Species (no.)</t>
+  </si>
+  <si>
+    <t>New High Species (perc.)</t>
+  </si>
+  <si>
+    <t>Trend New</t>
+  </si>
+  <si>
+    <t>Trend Different</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>IUCN</t>
+  </si>
+  <si>
+    <t>SOIB Concern Status</t>
+  </si>
+  <si>
+    <t>SOIBv2 Priority Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Critically Endangered</t>
+  </si>
+  <si>
+    <t>Endangered</t>
+  </si>
+  <si>
+    <t>Vulnerable</t>
+  </si>
+  <si>
+    <t>Near Threatened</t>
+  </si>
+  <si>
+    <t>Least Concern</t>
+  </si>
+  <si>
+    <t>Not Recognised</t>
+  </si>
+  <si>
+    <t>More decline in LTT</t>
+  </si>
+  <si>
+    <t>More decline in CAT</t>
+  </si>
+  <si>
+    <t>First-time trend</t>
+  </si>
+  <si>
+    <t>First-time LTT</t>
+  </si>
+  <si>
+    <t>First-time CAT</t>
+  </si>
+  <si>
+    <t>Other changes in trends</t>
+  </si>
+  <si>
+    <t>Loss of trends</t>
+  </si>
+  <si>
+    <t>Reducing range</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Less decline in LTT</t>
+  </si>
+  <si>
+    <t>Less decline in CAT</t>
+  </si>
+  <si>
+    <t>Increasing range</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +274,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -118,7 +326,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -152,6 +360,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -186,9 +395,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -361,45 +571,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Trend Status</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Long-term species (no.)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Current species (no.)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Long-term species conclusive (perc.)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Current species conclusive (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Rapid Decline</t>
-        </is>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>98</v>
@@ -414,11 +612,9 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Decline</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>106</v>
@@ -433,11 +629,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>98</v>
@@ -452,11 +646,9 @@
         <v>52.6</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
         <v>19</v>
@@ -471,11 +663,9 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Rapid Increase</t>
-        </is>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
         <v>17</v>
@@ -490,11 +680,9 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Trend Inconclusive</t>
-        </is>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
         <v>185</v>
@@ -503,11 +691,9 @@
         <v>284</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Insufficient Data</t>
-        </is>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
       <c r="B8">
         <v>419</v>
@@ -522,55 +708,47 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Critically Endangered</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Endangered</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Vulnerable</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Near Threatened</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Least Concern</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Not Recognised</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
       </c>
       <c r="B2">
         <v>7.9</v>
@@ -591,11 +769,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -613,14 +789,12 @@
         <v>83.3</v>
       </c>
       <c r="G3">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -638,7 +812,7 @@
         <v>95.7</v>
       </c>
       <c r="G4">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -647,35 +821,27 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Break-up</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Species (no.)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Species (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>More decline in LTT</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
       </c>
       <c r="B2">
         <v>22</v>
@@ -684,11 +850,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>More decline in CAT</t>
-        </is>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -697,11 +861,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>First-time trend</t>
-        </is>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -710,24 +872,20 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>First-time LTT</t>
-        </is>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>First-time CAT</t>
-        </is>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -736,37 +894,31 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other changes in trends</t>
-        </is>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Loss of trends</t>
-        </is>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Reducing range</t>
-        </is>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -775,11 +927,9 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Others</t>
-        </is>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -794,35 +944,27 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Break-up</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Species (no.)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Species (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Less decline in LTT</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -831,11 +973,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Less decline in CAT</t>
-        </is>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -844,11 +984,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>First-time trend</t>
-        </is>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -857,11 +995,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>First-time LTT</t>
-        </is>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -870,11 +1006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>First-time CAT</t>
-        </is>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -883,11 +1017,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other changes in trends</t>
-        </is>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -896,11 +1028,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Loss of trends</t>
-        </is>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -909,11 +1039,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Increasing range</t>
-        </is>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -922,11 +1050,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Others</t>
-        </is>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -941,35 +1067,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Range Status</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Species (no.)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Species (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Historical</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -978,24 +1096,20 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Very Restricted</t>
-        </is>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
       </c>
       <c r="B3">
         <v>46</v>
       </c>
       <c r="C3">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Restricted</t>
-        </is>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
       </c>
       <c r="B4">
         <v>220</v>
@@ -1004,11 +1118,9 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
       </c>
       <c r="B5">
         <v>363</v>
@@ -1017,24 +1129,20 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Large</t>
-        </is>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
       <c r="B6">
         <v>178</v>
       </c>
       <c r="C6">
-        <v>18.9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Very Large</t>
-        </is>
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
       </c>
       <c r="B7">
         <v>131</v>
@@ -1049,50 +1157,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Priority Status</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>No. of species</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
       </c>
       <c r="B2">
         <v>178</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="B3">
         <v>323</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
       </c>
       <c r="B4">
         <v>441</v>
@@ -1104,45 +1202,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>No. of species in:</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Selected for analysis</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>With conclusive trends</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>SoIB 2023 Assessment</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
       </c>
       <c r="B2">
         <v>942</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Long-term Analysis</t>
-        </is>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
       </c>
       <c r="B3">
         <v>523</v>
@@ -1151,11 +1239,9 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Current Analysis</t>
-        </is>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
       </c>
       <c r="B4">
         <v>643</v>
@@ -1164,11 +1250,9 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Range Analysis</t>
-        </is>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
       </c>
       <c r="B5">
         <v>942</v>
@@ -1180,45 +1264,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Break-up</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>High Species (no.)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>High Species (perc.)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>New High Species (no.)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>New High Species (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Trend New</t>
-        </is>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
       </c>
       <c r="B2">
         <v>77</v>
@@ -1233,11 +1312,9 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Trend Different</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
       </c>
       <c r="B3">
         <v>17</v>
@@ -1252,11 +1329,9 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Range</t>
-        </is>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
       </c>
       <c r="B4">
         <v>45</v>
@@ -1271,11 +1346,9 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>IUCN</t>
-        </is>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
       </c>
       <c r="B5">
         <v>39</v>
@@ -1296,45 +1369,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>SOIB Concern Status</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>SOIBv2 Priority Status</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Species (no.)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Species (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
       </c>
       <c r="C2">
         <v>74</v>
@@ -1343,16 +1404,12 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -1361,16 +1418,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
       <c r="C4">
         <v>22</v>
@@ -1379,11 +1432,9 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1392,16 +1443,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6">
         <v>32</v>
@@ -1410,16 +1457,12 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
       </c>
       <c r="C7">
         <v>333</v>
@@ -1428,16 +1471,12 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
       </c>
       <c r="C8">
         <v>72</v>
@@ -1446,11 +1485,9 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -1459,34 +1496,26 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10">
         <v>56</v>
       </c>
       <c r="D10">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
       </c>
       <c r="C11">
         <v>81</v>
@@ -1495,16 +1524,12 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
       <c r="C12">
         <v>166</v>
@@ -1513,11 +1538,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
       </c>
       <c r="C13">
         <v>16</v>
@@ -1532,45 +1555,33 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>SOIBv2 Priority Status</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>SOIB Concern Status</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Species (no.)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Species (perc.)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
       </c>
       <c r="C2">
         <v>74</v>
@@ -1579,16 +1590,12 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
       </c>
       <c r="C3">
         <v>32</v>
@@ -1597,16 +1604,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
       <c r="C4">
         <v>56</v>
@@ -1615,11 +1618,9 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1628,16 +1629,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1646,16 +1643,12 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
       </c>
       <c r="C7">
         <v>333</v>
@@ -1664,29 +1657,23 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
       </c>
       <c r="C8">
         <v>81</v>
       </c>
       <c r="D8">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
       </c>
       <c r="C9">
         <v>24</v>
@@ -1695,16 +1682,12 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10">
         <v>22</v>
@@ -1713,16 +1696,12 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
       </c>
       <c r="C11">
         <v>72</v>
@@ -1731,16 +1710,12 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
       <c r="C12">
         <v>166</v>
@@ -1749,11 +1724,9 @@
         <v>51.4</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
       </c>
       <c r="C13">
         <v>63</v>
@@ -1768,45 +1741,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Sum</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Critically Endangered</t>
-        </is>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -1821,11 +1782,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Endangered</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1840,11 +1799,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Vulnerable</t>
-        </is>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
       </c>
       <c r="B4">
         <v>42</v>
@@ -1859,11 +1816,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Near Threatened</t>
-        </is>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
       </c>
       <c r="B5">
         <v>17</v>
@@ -1878,11 +1833,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Least Concern</t>
-        </is>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="B6">
         <v>90</v>
@@ -1897,11 +1850,9 @@
         <v>781</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Not Recognised</t>
-        </is>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1916,11 +1867,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sum</t>
-        </is>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
       </c>
       <c r="B8">
         <v>178</v>
@@ -1941,40 +1890,33 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Moderate</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Critically Endangered</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1986,11 +1928,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Endangered</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
       </c>
       <c r="B3">
         <v>93.8</v>
@@ -2002,11 +1942,9 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Vulnerable</t>
-        </is>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
       </c>
       <c r="B4">
         <v>80.8</v>
@@ -2018,11 +1956,9 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Near Threatened</t>
-        </is>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
       </c>
       <c r="B5">
         <v>25.4</v>
@@ -2031,14 +1967,12 @@
         <v>58.2</v>
       </c>
       <c r="D5">
-        <v>16.4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Least Concern</t>
-        </is>
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="B6">
         <v>11.5</v>
@@ -2050,11 +1984,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Not Recognised</t>
-        </is>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
       </c>
       <c r="B7">
         <v>0</v>

</xml_diff>

<commit_message>
I went back a few steps by undoing some commits because there was a problem while pushing. I used this command git reset --soft HEAD~3
But I used it 3 times by mistake!

Now I'm recommitting everything, hope everything remains fine.
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="11_731CB15E13ABE5F5B7A6A05411BB4C0B1FE5DA23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50130536-ED49-440D-8F35-3199A8212709}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trends Status" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -947,7 +947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1205,7 +1207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Results generated after correcting error estimation and the number of projected years.
There are not final results though because the trends have not been rerun after the filtering bug fix.
</commit_message>
<xml_diff>
--- a/01_analyses_full/results/SoIB_summaries.xlsx
+++ b/01_analyses_full/results/SoIB_summaries.xlsx
@@ -410,16 +410,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D2">
-        <v>15.7</v>
+        <v>16.7</v>
       </c>
       <c r="E2">
-        <v>8.699999999999999</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="3">
@@ -429,16 +429,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C3">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D3">
-        <v>22.5</v>
+        <v>25.9</v>
       </c>
       <c r="E3">
-        <v>27.8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -448,16 +448,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D4">
-        <v>35.8</v>
+        <v>32.5</v>
       </c>
       <c r="E4">
-        <v>50.6</v>
+        <v>48.3</v>
       </c>
     </row>
     <row r="5">
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>12.3</v>
+        <v>11.4</v>
       </c>
       <c r="E5">
-        <v>7.1</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="6">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>13.7</v>
+        <v>13.6</v>
       </c>
       <c r="E6">
-        <v>5.8</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="C7">
-        <v>410</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8">
@@ -833,10 +833,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>12.5</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="3">
@@ -846,10 +846,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>13.8</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="4">
@@ -898,10 +898,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>13.8</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="8">
@@ -911,10 +911,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="9">
@@ -2467,7 +2467,7 @@
         <v>526</v>
       </c>
       <c r="C3">
-        <v>204</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4">
@@ -2480,7 +2480,7 @@
         <v>651</v>
       </c>
       <c r="C4">
-        <v>241</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5">

</xml_diff>